<commit_message>
add more Chord tone.
</commit_message>
<xml_diff>
--- a/Document/Harmonics Study/Chord Scale.xlsx
+++ b/Document/Harmonics Study/Chord Scale.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="78">
   <si>
     <t>Chord</t>
   </si>
@@ -162,6 +162,170 @@
   </si>
   <si>
     <t>CM7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S 11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FM7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FM7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dominant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tb9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T#9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tb13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>♭A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>♭E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T#11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Leading</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bm7(b5)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bm7(b5)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S 11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tb13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tb9</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -169,7 +333,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,24 +350,152 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="16"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF9C6500"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -354,10 +646,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -366,68 +658,363 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
       <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -441,7 +1028,29 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -451,86 +1060,333 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="16" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="17" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="20" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="19" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="16" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="17" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="39" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="38" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="39" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="38" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="41" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="27" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="28" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="29" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="44" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="45" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="31" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="32" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="23" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="25" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="24" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="42" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="43" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="21" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="37" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="36" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="37" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="36" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="40" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="22" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="24" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="26" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="22" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="24" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="26" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="18" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="30" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="12">
+    <cellStyle name="60% - 강조색1" xfId="5" builtinId="32"/>
+    <cellStyle name="60% - 강조색2" xfId="7" builtinId="36"/>
+    <cellStyle name="60% - 강조색4" xfId="9" builtinId="44"/>
+    <cellStyle name="60% - 강조색5" xfId="11" builtinId="48"/>
+    <cellStyle name="강조색1" xfId="4" builtinId="29"/>
+    <cellStyle name="강조색2" xfId="6" builtinId="33"/>
+    <cellStyle name="강조색4" xfId="8" builtinId="41"/>
+    <cellStyle name="강조색5" xfId="10" builtinId="45"/>
+    <cellStyle name="계산" xfId="2" builtinId="22"/>
+    <cellStyle name="메모" xfId="3" builtinId="10"/>
+    <cellStyle name="보통" xfId="1" builtinId="28"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -830,200 +1686,201 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C6:M16"/>
+  <dimension ref="C6:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="0.83203125" style="1" customWidth="1"/>
-    <col min="2" max="4" width="8.6640625" style="1"/>
+    <col min="2" max="2" width="8.4140625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="8.6640625" style="1"/>
     <col min="5" max="13" width="5.58203125" style="1" customWidth="1"/>
     <col min="14" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="7" spans="3:13" ht="26" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D7" s="2" t="s">
+    <row r="7" spans="3:13" ht="21.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D7" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="7" t="s">
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="17"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="16" t="s">
+      <c r="J7" s="21"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="M7" s="18"/>
+      <c r="M7" s="22"/>
     </row>
     <row r="8" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="19"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="25"/>
     </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="C9" s="1" t="s">
+    <row r="9" spans="3:13" s="56" customFormat="1" ht="17.5" x14ac:dyDescent="0.45">
+      <c r="C9" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="J9" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="K9" s="5"/>
-      <c r="L9" s="10" t="s">
+      <c r="K9" s="62"/>
+      <c r="L9" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="5"/>
+      <c r="M9" s="64"/>
     </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="D10" s="14" t="s">
+    <row r="10" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D10" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="11">
         <v>1</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="11">
         <v>5</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="H10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="15"/>
-      <c r="L10" s="14" t="s">
+      <c r="K10" s="31"/>
+      <c r="L10" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="M10" s="15"/>
+      <c r="M10" s="28"/>
     </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="D11" s="14" t="s">
+    <row r="11" spans="3:13" s="56" customFormat="1" ht="17.5" x14ac:dyDescent="0.45">
+      <c r="D11" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="14" t="s">
+      <c r="J11" s="66"/>
+      <c r="K11" s="62"/>
+      <c r="L11" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="M11" s="68" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="D12" s="14" t="s">
+    <row r="12" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D12" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="11">
         <v>1</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="11">
         <v>5</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="14" t="s">
+      <c r="J12" s="33"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="M12" s="15" t="s">
+      <c r="M12" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="D13" s="14" t="s">
+    <row r="13" spans="3:13" s="56" customFormat="1" ht="17.5" x14ac:dyDescent="0.45">
+      <c r="D13" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H13" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="I13" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J13" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="K13" s="15" t="s">
+      <c r="K13" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="L13" s="14"/>
-      <c r="M13" s="15"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="51"/>
     </row>
     <row r="14" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="27" t="s">
         <v>35</v>
       </c>
       <c r="E14" s="13">
@@ -1035,40 +1892,328 @@
       <c r="G14" s="13">
         <v>5</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J14" s="13" t="s">
+      <c r="J14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="K14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L14" s="12"/>
-      <c r="M14" s="6"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="53"/>
     </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="C15" s="1" t="s">
+    <row r="15" spans="3:13" s="56" customFormat="1" ht="17.5" x14ac:dyDescent="0.45">
+      <c r="C15" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="57" t="s">
         <v>36</v>
       </c>
+      <c r="E15" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="75" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="J15" s="61" t="s">
+        <v>42</v>
+      </c>
+      <c r="K15" s="62"/>
+      <c r="L15" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="M15" s="64"/>
     </row>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="D16" s="1" t="s">
+    <row r="16" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D16" s="26" t="s">
         <v>36</v>
       </c>
+      <c r="E16" s="11">
+        <v>1</v>
+      </c>
+      <c r="F16" s="11">
+        <v>3</v>
+      </c>
+      <c r="G16" s="11">
+        <v>5</v>
+      </c>
+      <c r="H16" s="15">
+        <v>7</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J16" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="K16" s="31"/>
+      <c r="L16" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="M16" s="28"/>
+    </row>
+    <row r="17" spans="3:13" s="56" customFormat="1" ht="17.5" x14ac:dyDescent="0.45">
+      <c r="D17" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="70" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" s="76" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" s="73" t="s">
+        <v>52</v>
+      </c>
+      <c r="K17" s="74" t="s">
+        <v>53</v>
+      </c>
+      <c r="L17" s="50"/>
+      <c r="M17" s="51"/>
+    </row>
+    <row r="18" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D18" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="13">
+        <v>1</v>
+      </c>
+      <c r="F18" s="13">
+        <v>3</v>
+      </c>
+      <c r="G18" s="13">
+        <v>5</v>
+      </c>
+      <c r="H18" s="16">
+        <v>7</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K18" s="5">
+        <v>13</v>
+      </c>
+      <c r="L18" s="52"/>
+      <c r="M18" s="53"/>
+    </row>
+    <row r="19" spans="3:13" s="56" customFormat="1" ht="17.5" x14ac:dyDescent="0.45">
+      <c r="C19" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" s="60" t="s">
+        <v>42</v>
+      </c>
+      <c r="J19" s="77" t="s">
+        <v>62</v>
+      </c>
+      <c r="K19" s="78" t="s">
+        <v>61</v>
+      </c>
+      <c r="L19" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="M19" s="45"/>
+    </row>
+    <row r="20" spans="3:13" s="56" customFormat="1" ht="17.5" x14ac:dyDescent="0.45">
+      <c r="D20" s="55"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="79" t="s">
+        <v>38</v>
+      </c>
+      <c r="J20" s="80" t="s">
+        <v>63</v>
+      </c>
+      <c r="K20" s="81" t="s">
+        <v>65</v>
+      </c>
+      <c r="L20" s="48"/>
+      <c r="M20" s="49"/>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.45">
+      <c r="D21" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="17">
+        <v>1</v>
+      </c>
+      <c r="F21" s="17">
+        <v>3</v>
+      </c>
+      <c r="G21" s="17">
+        <v>5</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="L21" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="M21" s="39"/>
+    </row>
+    <row r="22" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D22" s="35"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L22" s="40"/>
+      <c r="M22" s="41"/>
+    </row>
+    <row r="23" spans="3:13" s="56" customFormat="1" ht="17.5" x14ac:dyDescent="0.45">
+      <c r="C23" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="G23" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="H23" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="I23" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="K23" s="62"/>
+      <c r="L23" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="M23" s="64"/>
+    </row>
+    <row r="24" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D24" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="11">
+        <v>1</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J24" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="K24" s="31"/>
+      <c r="L24" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="M24" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="32">
+    <mergeCell ref="L21:M22"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="L13:M14"/>
+    <mergeCell ref="L17:M18"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="L19:M20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
     <mergeCell ref="E7:H7"/>
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="D8:M8"/>
     <mergeCell ref="L7:M7"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="L15:M15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>